<commit_message>
Fix issues with TestEnvironmentConfig
1. Add has null for password and username parameters
2. Add sample testCase
</commit_message>
<xml_diff>
--- a/src/main/resources/CompilerDictionary/LocatorDictionary/LocatorDictionary1.xlsx
+++ b/src/main/resources/CompilerDictionary/LocatorDictionary/LocatorDictionary1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gurcharan/Desktop/Mobile-Web-Browser-Automation/src/main/resources/CompilerDictionary/LocatorDictionary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1058B743-39B3-394C-9530-3751DA13F487}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC02AC50-21D0-4541-8A22-5C4B33C95D46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="680" windowWidth="30240" windowHeight="17700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="680" windowWidth="30240" windowHeight="17560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BecomePartnerPage" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
   <si>
     <t>Sno</t>
   </si>
@@ -34,6 +34,42 @@
   </si>
   <si>
     <t>Locator Type</t>
+  </si>
+  <si>
+    <t>Guru99_TestBank_Header</t>
+  </si>
+  <si>
+    <t>h2.barone</t>
+  </si>
+  <si>
+    <t>CSS</t>
+  </si>
+  <si>
+    <t>table tr td[align='right']</t>
+  </si>
+  <si>
+    <t>input[name='emailid']</t>
+  </si>
+  <si>
+    <t>input[type='submit']</t>
+  </si>
+  <si>
+    <t>Guru99_TestBank_Button_Submit</t>
+  </si>
+  <si>
+    <t>Guru99_TestBank_TextBox_Email</t>
+  </si>
+  <si>
+    <t>Guru99_TestBank_Label_Email</t>
+  </si>
+  <si>
+    <t>//h2[text()='Access details to demo site.']</t>
+  </si>
+  <si>
+    <t>Xpath</t>
+  </si>
+  <si>
+    <t>Guru99_TestBank_AccessDetailsToDemoSite</t>
   </si>
 </sst>
 </file>
@@ -384,10 +420,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -416,6 +452,96 @@
       <c r="A2">
         <v>1</v>
       </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>10</v>
+      </c>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:C38">

</xml_diff>